<commit_message>
News & order form added
</commit_message>
<xml_diff>
--- a/xls/zavazna-objednavka.xlsx
+++ b/xls/zavazna-objednavka.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="20115" windowHeight="10995" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="20115" windowHeight="10935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moduly" sheetId="3" r:id="rId1"/>
@@ -21,12 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Pro podniky</t>
-  </si>
-  <si>
-    <t>Učebnice a přístup k 10 lekcím v online pracovním sešitu pro jednoho studenta</t>
   </si>
   <si>
     <t>Naše moduly:</t>
@@ -173,19 +170,10 @@
     <t>Služby v cestovním ruchu, odborná němčina</t>
   </si>
   <si>
-    <t>Výuka cizích jazyků se zaměřením na odborné předměty středních škol, kurz akreditovaný MŠMT v rámci v systému DVPP pod č.j.: MŠMT -17744/2014-1-561. Kurz může probíhat přímo u Vás minimálně pro 6 a maximálně 8 účastníků, v ceně kurzu je online kurz, k němu učebnice a online podpora lektora, metodický kurz, k němu příručka pro lektora.</t>
-  </si>
-  <si>
-    <t>Metodický kurz</t>
-  </si>
-  <si>
     <t>Vyplněný objednávkový formulář pošlete ve formátu PDF na dehner@openagency.cz nebo poštou.</t>
   </si>
   <si>
     <t>Jméno kontaktní osoby:</t>
-  </si>
-  <si>
-    <t>poštovné</t>
   </si>
   <si>
     <t>Výuka s certifikovaným lektorem pro 2-6 účastníků v rozsahu 40 hodin á 45 minut</t>
@@ -202,16 +190,37 @@
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t>2300539840/2010</t>
+      <t xml:space="preserve">2300539840/2010 </t>
+    </r>
+  </si>
+  <si>
+    <t>Metodický kurz / Workshop (Teachers Training)</t>
+  </si>
+  <si>
+    <t>Výuka cizích jazyků se zaměřením na odborné/přírodovědné předměty středních/základních škol. Kurz akreditovaný MŠMT v rámci v systému DVPP</t>
+  </si>
+  <si>
+    <t>Setkání učitelů a lektorů OPEN LEARNING</t>
+  </si>
+  <si>
+    <t>Učebnice a přístup na 10 měsíců k online pracovnímu sešitu/1 žák</t>
+  </si>
+  <si>
+    <t>Učebnice a přístup k 10 lekcím v online pracovním sešitu pro jednoho účastníka</t>
+  </si>
+  <si>
+    <r>
+      <t>Učebnice a přístup na 10 měsíců k online pracovnímu sešitu/1 žák                                  *</t>
     </r>
     <r>
       <rPr>
+        <i/>
         <sz val="11"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t>.</t>
+      <t>Při nákupu pro 20 a více žáků</t>
     </r>
   </si>
 </sst>
@@ -270,7 +279,9 @@
       <charset val="238"/>
     </font>
     <font>
-      <sz val="12"/>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
@@ -308,7 +319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -378,21 +389,6 @@
       </top>
       <bottom style="double">
         <color rgb="FFCCFF99"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF79C6FF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF79C6FF"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -662,51 +658,76 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF79C6FF"/>
       </left>
       <right style="thin">
         <color rgb="FF79C6FF"/>
       </right>
+      <top style="thin">
+        <color rgb="FF79C6FF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF79C6FF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF79C6FF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF79C6FF"/>
+      </right>
       <top style="double">
         <color theme="1"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF79C6FF"/>
-      </left>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF79C6FF"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF79C6FF"/>
+      </right>
+      <top/>
       <bottom style="double">
         <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -717,132 +738,157 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1199,10 +1245,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="List3"/>
-  <dimension ref="A2:B17"/>
+  <dimension ref="A2:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B3:B17"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1214,80 +1260,85 @@
     <row r="2" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
-        <v>41</v>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="61" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1299,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:G44"/>
+  <dimension ref="B8:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="80" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1312,365 +1363,380 @@
     <col min="3" max="3" width="47.140625" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="37" customWidth="1"/>
     <col min="7" max="7" width="1.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="8" spans="2:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="B8" s="38" t="s">
-        <v>28</v>
+      <c r="B8" s="31" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="37" t="s">
-        <v>30</v>
+      <c r="C10" s="30" t="s">
+        <v>29</v>
       </c>
       <c r="D10" s="52"/>
       <c r="E10" s="53"/>
-      <c r="G10" s="30"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="37" t="s">
-        <v>29</v>
+      <c r="C11" s="30" t="s">
+        <v>28</v>
       </c>
       <c r="D11" s="52"/>
       <c r="E11" s="53"/>
-      <c r="G11" s="30"/>
+      <c r="G11" s="24"/>
     </row>
     <row r="12" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="37" t="s">
-        <v>31</v>
+      <c r="C12" s="30" t="s">
+        <v>30</v>
       </c>
       <c r="D12" s="52"/>
       <c r="E12" s="53"/>
-      <c r="G12" s="30"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="13" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="37" t="s">
-        <v>32</v>
+      <c r="C13" s="30" t="s">
+        <v>31</v>
       </c>
       <c r="D13" s="52"/>
       <c r="E13" s="53"/>
     </row>
     <row r="14" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="37" t="s">
-        <v>45</v>
+      <c r="C14" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="D14" s="52"/>
       <c r="E14" s="53"/>
     </row>
     <row r="15" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="52"/>
+      <c r="C15" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="54"/>
       <c r="E15" s="53"/>
     </row>
     <row r="16" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
     </row>
     <row r="17" spans="2:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="D17" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="F17" s="38" t="s">
         <v>22</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B18" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="42">
+      <c r="C18" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="35">
         <v>690</v>
       </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
-      <c r="C19" s="32" t="s">
+      <c r="B19" s="50"/>
+      <c r="C19" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="34">
+        <v>23400</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="40"/>
+    </row>
+    <row r="20" spans="2:6" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="33">
+        <v>990</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="41"/>
+    </row>
+    <row r="21" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B21" s="49"/>
+      <c r="C21" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="32">
+        <v>300</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="42"/>
+    </row>
+    <row r="22" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="50"/>
+      <c r="C22" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="34">
+        <v>6000</v>
+      </c>
+      <c r="E22" s="28"/>
+      <c r="F22" s="40"/>
+    </row>
+    <row r="23" spans="2:6" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="33">
+        <v>990</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="41"/>
+    </row>
+    <row r="24" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B24" s="59"/>
+      <c r="C24" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="32">
+        <v>300</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="43"/>
+    </row>
+    <row r="25" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B25" s="59"/>
+      <c r="C25" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="32">
+        <v>1490</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="F25" s="43"/>
+    </row>
+    <row r="26" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B26" s="59"/>
+      <c r="C26" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="32">
+        <v>110</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="43"/>
+    </row>
+    <row r="27" spans="2:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="B27" s="59"/>
+      <c r="C27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="32">
+        <v>3460</v>
+      </c>
+      <c r="E27" s="18"/>
+      <c r="F27" s="43"/>
+    </row>
+    <row r="28" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B28" s="59"/>
+      <c r="C28" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="41">
-        <v>23400</v>
-      </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35"/>
-    </row>
-    <row r="20" spans="2:6" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="40">
-        <v>990</v>
-      </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
-    </row>
-    <row r="21" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="46"/>
-      <c r="C21" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="39">
+      <c r="D28" s="57">
         <v>300</v>
       </c>
-      <c r="E21" s="22"/>
-      <c r="F21" s="19"/>
-    </row>
-    <row r="22" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
-      <c r="C22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="41">
-        <v>6000</v>
-      </c>
-      <c r="E22" s="34"/>
-      <c r="F22" s="35"/>
-    </row>
-    <row r="23" spans="2:6" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="40">
-        <v>990</v>
-      </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
-    </row>
-    <row r="24" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B24" s="49"/>
-      <c r="C24" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="39">
-        <v>300</v>
-      </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="23"/>
-    </row>
-    <row r="25" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B25" s="49"/>
-      <c r="C25" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="39">
-        <v>1490</v>
-      </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="23"/>
-    </row>
-    <row r="26" spans="2:6" ht="114" x14ac:dyDescent="0.2">
-      <c r="B26" s="49"/>
-      <c r="C26" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="39">
-        <v>3460</v>
-      </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="23"/>
-    </row>
-    <row r="27" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B27" s="49"/>
-      <c r="C27" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="39">
-        <v>300</v>
-      </c>
-      <c r="E27" s="22"/>
-      <c r="F27" s="23"/>
-    </row>
-    <row r="28" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="50"/>
-      <c r="C28" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="41">
+      <c r="E28" s="55"/>
+      <c r="F28" s="56"/>
+    </row>
+    <row r="29" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B29" s="59"/>
+      <c r="C29" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="57">
         <v>690</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
-    </row>
-    <row r="29" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="34"/>
-      <c r="C29" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="33">
-        <v>64</v>
-      </c>
-      <c r="E29" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="F29" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="56"/>
+    </row>
+    <row r="30" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="60"/>
+      <c r="C30" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="34">
+        <v>590</v>
+      </c>
+      <c r="E30" s="28"/>
+      <c r="F30" s="40"/>
     </row>
     <row r="31" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="25">
-        <f>IF(F18+F19+F22+F24+F27+F28&gt;=10,D18*F18+D19*F19+D20*F20+D21*F21+D22*F22+D23*F23+D24*F24+D27*F27+D28*F28,IF(F18+F19+F20+F21+F22+F23+F24+F27+F28=0,0,IF(F18+F19+F21+F24+F27+F28=0,D20*F20+D22*F22+D23*F23,D18*F18+D19*F19+D20*F20+D21*F21+D22*F22+D23*F23+D24*F24+D27*F27+D28*F28+D26*F26+D29)))</f>
+      <c r="C31" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="27">
+        <v>64</v>
+      </c>
+      <c r="E31" s="36"/>
+      <c r="F31" s="40"/>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="44"/>
+    </row>
+    <row r="33" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="6"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="45">
+        <f>D18*F18+D19*F19+D20*F20+D21*F21+D22*F22+D23*F23+D24*F24+D25*F25+D26*F26+D27*F27+D28*F28+D29*F29+D30*F30+F31*D31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B33" s="54" t="s">
+    <row r="34" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B36" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B34" s="55"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B35" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="3"/>
+      <c r="F38" s="46"/>
       <c r="G38" s="3"/>
     </row>
     <row r="39" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="3"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="46"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>37</v>
-      </c>
+    <row r="40" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="6"/>
-      <c r="F40" s="3"/>
+      <c r="F40" s="46"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B41" s="3"/>
-      <c r="C41" s="13" t="s">
+    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="11" t="s">
         <v>35</v>
       </c>
+      <c r="C41" s="3"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="3"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="46"/>
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="3"/>
       <c r="E42" s="6"/>
-      <c r="F42" s="3"/>
+      <c r="F42" s="46"/>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
+      <c r="C43" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="3"/>
       <c r="E43" s="6"/>
-      <c r="F43" s="3"/>
+      <c r="F43" s="46"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="28"/>
+    <row r="44" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B45" s="47"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="22"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B44:F44"/>
+  <mergeCells count="9">
     <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B28"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
@@ -1678,22 +1744,35 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B23:B30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E29">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E31">
       <formula1>Modul</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E18:E28">
-      <formula1>Moduly1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" scale="52" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Moduly!$B$3:$B$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>E30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Moduly!$B$3:$B$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>E18 E19 E20 E21 E22 E23 E24 E25 E26 E27 E28 E29</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>